<commit_message>
added match type setting
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\schedule_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8CC2B62A-8173-4BBD-8709-3EF223154D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35792C39-C97B-403E-90D0-24E8F15CA6EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="65">
   <si>
     <t>Team</t>
   </si>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1122,12 +1122,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H30" sqref="H30"/>
+      <selection pane="topRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1235,82 +1235,82 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="I2" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="J2" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="L2" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="M2" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="N2" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="O2" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="P2" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="Q2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="R2" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="S2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="T2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="U2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="V2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="W2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="X2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="Y2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="Z2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AA2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AB2" t="s">
         <v>59</v>
@@ -1333,82 +1333,82 @@
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="H3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="M3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="O3" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="P3" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="Q3" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="R3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="S3" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="T3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="U3" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="V3" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="W3" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="X3" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="Y3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="Z3" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="AA3" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="AB3" t="s">
         <v>59</v>
@@ -1431,82 +1431,82 @@
         <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="H4" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="J4" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="K4" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="L4" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="M4" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="N4" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="O4" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="P4" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="Q4" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="R4" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="S4" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="T4" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="U4" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="V4" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="W4" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="X4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="Y4" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="Z4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="AA4" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="AB4" t="s">
         <v>59</v>
@@ -1529,82 +1529,82 @@
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="H5" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="I5" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="J5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="K5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="L5" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="M5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="N5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="S5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="T5" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="U5" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="V5" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="W5" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="X5" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="Y5" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="Z5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="AA5" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="AB5" t="s">
         <v>59</v>
@@ -1627,82 +1627,82 @@
         <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="J6" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="K6" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="L6" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="M6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="N6" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="O6" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="P6" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="Q6" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="R6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="S6" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="T6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="U6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="V6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="W6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Y6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Z6" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="AA6" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="AB6" t="s">
         <v>59</v>
@@ -1725,82 +1725,82 @@
         <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="J7" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="K7" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="L7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="M7" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="N7" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="O7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="P7" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="Q7" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="R7" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="S7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="T7" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="U7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="V7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="W7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="X7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Z7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AA7" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="AB7" t="s">
         <v>59</v>
@@ -1823,82 +1823,82 @@
         <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G8" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="I8" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="J8" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="K8" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="L8" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="M8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Q8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="R8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="S8" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="T8" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="U8" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="V8" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="W8" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="X8" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="Y8" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="Z8" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="AA8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="AB8" t="s">
         <v>59</v>
@@ -1921,82 +1921,82 @@
         <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="H9" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="I9" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="J9" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="K9" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="L9" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="M9" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="N9" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="O9" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="P9" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="Q9" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="R9" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="S9" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="T9" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="U9" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="V9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="W9" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="X9" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="Y9" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="Z9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="AA9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="AB9" t="s">
         <v>59</v>
@@ -2019,82 +2019,82 @@
         <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="H10" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="I10" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="J10" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="K10" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="L10" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="M10" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="N10" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="O10" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="P10" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="Q10" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="R10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="U10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="V10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="W10" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="X10" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="Y10" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Z10" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="AA10" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="AB10" t="s">
         <v>59</v>
@@ -2117,82 +2117,82 @@
         <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="H11" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="I11" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="J11" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="K11" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="L11" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="M11" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="N11" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="O11" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="P11" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="Q11" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="R11" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="S11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="T11" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="U11" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="V11" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="W11" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="X11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Y11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AA11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="AB11" t="s">
         <v>59</v>
@@ -2215,82 +2215,82 @@
         <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G12" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="H12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I12" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="J12" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="K12" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="L12" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="M12" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="N12" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="O12" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="P12" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q12" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="R12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="S12" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="T12" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="U12" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="V12" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="W12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X12" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="Y12" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="Z12" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="AA12" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="AB12" t="s">
         <v>59</v>
@@ -2313,82 +2313,82 @@
         <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G13" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="H13" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="I13" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="J13" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="K13" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="L13" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="M13" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="N13" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="O13" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="P13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Q13" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="R13" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="S13" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="T13" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="U13" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="V13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W13" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="X13" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="Y13" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="Z13" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="AA13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AB13" t="s">
         <v>59</v>
@@ -2411,76 +2411,82 @@
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="G14" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="H14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="N14" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="O14" t="s">
-        <v>34</v>
+        <v>59</v>
+      </c>
+      <c r="P14" t="s">
+        <v>59</v>
       </c>
       <c r="Q14" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="R14" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="S14" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="T14" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="U14" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="V14" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="W14" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="X14" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="Y14" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="Z14" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>59</v>
       </c>
       <c r="AB14" t="s">
         <v>59</v>
@@ -2502,41 +2508,83 @@
       <c r="A15" t="s">
         <v>55</v>
       </c>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="G15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" t="s">
+        <v>59</v>
       </c>
       <c r="J15" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="K15" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="L15" t="s">
+        <v>59</v>
+      </c>
+      <c r="M15" t="s">
+        <v>59</v>
+      </c>
+      <c r="N15" t="s">
+        <v>59</v>
+      </c>
+      <c r="O15" t="s">
+        <v>59</v>
+      </c>
+      <c r="P15" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>59</v>
       </c>
       <c r="R15" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="S15" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="T15" t="s">
+        <v>59</v>
       </c>
       <c r="U15" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="V15" t="s">
+        <v>59</v>
       </c>
       <c r="W15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="X15" t="s">
-        <v>32</v>
+        <v>59</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>59</v>
       </c>
       <c r="Z15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AA15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AB15" t="s">
         <v>59</v>
@@ -2558,38 +2606,83 @@
       <c r="A16" t="s">
         <v>62</v>
       </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="G16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" t="s">
+        <v>59</v>
+      </c>
+      <c r="J16" t="s">
+        <v>59</v>
+      </c>
+      <c r="K16" t="s">
+        <v>59</v>
       </c>
       <c r="L16" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="M16" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="N16" t="s">
+        <v>59</v>
+      </c>
+      <c r="O16" t="s">
+        <v>59</v>
       </c>
       <c r="P16" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="Q16" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="R16" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="S16" t="s">
+        <v>59</v>
+      </c>
+      <c r="T16" t="s">
+        <v>59</v>
       </c>
       <c r="U16" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+      <c r="V16" t="s">
+        <v>59</v>
+      </c>
+      <c r="W16" t="s">
+        <v>59</v>
+      </c>
+      <c r="X16" t="s">
+        <v>59</v>
       </c>
       <c r="Y16" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>59</v>
       </c>
       <c r="AA16" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="AB16" t="s">
         <v>59</v>
@@ -2611,44 +2704,83 @@
       <c r="A17" t="s">
         <v>41</v>
       </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="F17" t="s">
+        <v>59</v>
       </c>
       <c r="G17" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="H17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" t="s">
+        <v>59</v>
       </c>
       <c r="J17" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="K17" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="L17" t="s">
+        <v>59</v>
       </c>
       <c r="M17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N17" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="O17" t="s">
+        <v>59</v>
       </c>
       <c r="P17" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>59</v>
+      </c>
+      <c r="R17" t="s">
+        <v>59</v>
+      </c>
+      <c r="S17" t="s">
+        <v>59</v>
+      </c>
+      <c r="T17" t="s">
+        <v>59</v>
+      </c>
+      <c r="U17" t="s">
+        <v>59</v>
       </c>
       <c r="V17" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="W17" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="X17" t="s">
+        <v>59</v>
       </c>
       <c r="Y17" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="Z17" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="AA17" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="AB17" t="s">
         <v>59</v>
@@ -2671,40 +2803,82 @@
         <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="G18" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" t="s">
+        <v>59</v>
       </c>
       <c r="J18" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="K18" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" t="s">
+        <v>59</v>
+      </c>
+      <c r="M18" t="s">
+        <v>59</v>
       </c>
       <c r="N18" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="O18" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="P18" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>59</v>
+      </c>
+      <c r="R18" t="s">
+        <v>59</v>
       </c>
       <c r="S18" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="T18" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="U18" t="s">
+        <v>59</v>
+      </c>
+      <c r="V18" t="s">
+        <v>59</v>
       </c>
       <c r="W18" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+      <c r="X18" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>59</v>
       </c>
       <c r="Z18" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AA18" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="AB18" t="s">
         <v>59</v>
@@ -2727,37 +2901,82 @@
         <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="F19" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" t="s">
+        <v>59</v>
       </c>
       <c r="H19" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="I19" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="J19" t="s">
+        <v>59</v>
       </c>
       <c r="K19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L19" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="M19" t="s">
+        <v>59</v>
+      </c>
+      <c r="N19" t="s">
+        <v>59</v>
+      </c>
+      <c r="O19" t="s">
+        <v>59</v>
+      </c>
+      <c r="P19" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>59</v>
+      </c>
+      <c r="R19" t="s">
+        <v>59</v>
+      </c>
+      <c r="S19" t="s">
+        <v>59</v>
       </c>
       <c r="T19" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="U19" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="V19" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="W19" t="s">
+        <v>59</v>
+      </c>
+      <c r="X19" t="s">
+        <v>59</v>
       </c>
       <c r="Y19" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>59</v>
       </c>
       <c r="AB19" t="s">
         <v>59</v>
@@ -2780,34 +2999,82 @@
         <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="G20" t="s">
+        <v>59</v>
       </c>
       <c r="H20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I20" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="J20" t="s">
+        <v>59</v>
+      </c>
+      <c r="K20" t="s">
+        <v>59</v>
+      </c>
+      <c r="L20" t="s">
+        <v>59</v>
+      </c>
+      <c r="M20" t="s">
+        <v>59</v>
+      </c>
+      <c r="N20" t="s">
+        <v>59</v>
+      </c>
+      <c r="O20" t="s">
+        <v>59</v>
       </c>
       <c r="P20" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>59</v>
       </c>
       <c r="R20" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="S20" t="s">
+        <v>59</v>
+      </c>
+      <c r="T20" t="s">
+        <v>59</v>
+      </c>
+      <c r="U20" t="s">
+        <v>59</v>
       </c>
       <c r="V20" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="W20" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="X20" t="s">
+        <v>59</v>
       </c>
       <c r="Y20" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>59</v>
       </c>
       <c r="AB20" t="s">
         <v>59</v>
@@ -2830,40 +3097,82 @@
         <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" t="s">
+        <v>59</v>
       </c>
       <c r="G21" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="H21" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="I21" t="s">
+        <v>59</v>
+      </c>
+      <c r="J21" t="s">
+        <v>59</v>
       </c>
       <c r="K21" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+      <c r="L21" t="s">
+        <v>59</v>
+      </c>
+      <c r="M21" t="s">
+        <v>59</v>
       </c>
       <c r="N21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="O21" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="P21" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="Q21" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="R21" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="S21" t="s">
+        <v>59</v>
+      </c>
+      <c r="T21" t="s">
+        <v>59</v>
       </c>
       <c r="U21" t="s">
-        <v>32</v>
+        <v>59</v>
+      </c>
+      <c r="V21" t="s">
+        <v>59</v>
+      </c>
+      <c r="W21" t="s">
+        <v>59</v>
       </c>
       <c r="X21" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>59</v>
       </c>
       <c r="AB21" t="s">
         <v>59</v>
@@ -2885,38 +3194,83 @@
       <c r="A22" t="s">
         <v>34</v>
       </c>
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="E22" t="s">
+        <v>59</v>
       </c>
       <c r="F22" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G22" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="H22" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" t="s">
+        <v>59</v>
+      </c>
+      <c r="J22" t="s">
+        <v>59</v>
+      </c>
+      <c r="K22" t="s">
+        <v>59</v>
       </c>
       <c r="L22" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="M22" t="s">
+        <v>59</v>
+      </c>
+      <c r="N22" t="s">
+        <v>59</v>
       </c>
       <c r="O22" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="P22" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>59</v>
+      </c>
+      <c r="R22" t="s">
+        <v>59</v>
+      </c>
+      <c r="S22" t="s">
+        <v>59</v>
       </c>
       <c r="T22" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="U22" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="V22" t="s">
+        <v>59</v>
+      </c>
+      <c r="W22" t="s">
+        <v>59</v>
       </c>
       <c r="X22" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>59</v>
       </c>
       <c r="AA22" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="AB22" t="s">
         <v>59</v>
@@ -2938,38 +3292,83 @@
       <c r="A23" t="s">
         <v>48</v>
       </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" t="s">
+        <v>59</v>
       </c>
       <c r="G23" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+      <c r="H23" t="s">
+        <v>59</v>
       </c>
       <c r="I23" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="J23" t="s">
+        <v>59</v>
       </c>
       <c r="K23" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="L23" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="M23" t="s">
+        <v>59</v>
       </c>
       <c r="N23" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="O23" t="s">
+        <v>59</v>
+      </c>
+      <c r="P23" t="s">
+        <v>59</v>
       </c>
       <c r="Q23" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="R23" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="S23" t="s">
+        <v>59</v>
       </c>
       <c r="T23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="U23" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="V23" t="s">
+        <v>59</v>
+      </c>
+      <c r="W23" t="s">
+        <v>59</v>
+      </c>
+      <c r="X23" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>59</v>
       </c>
       <c r="AB23" t="s">
         <v>59</v>
@@ -2992,37 +3391,82 @@
         <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="D24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" t="s">
+        <v>59</v>
       </c>
       <c r="F24" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="G24" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="H24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I24" t="s">
+        <v>59</v>
       </c>
       <c r="J24" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="K24" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="L24" t="s">
+        <v>59</v>
       </c>
       <c r="M24" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="N24" t="s">
+        <v>59</v>
+      </c>
+      <c r="O24" t="s">
+        <v>59</v>
       </c>
       <c r="P24" t="s">
-        <v>32</v>
+        <v>59</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>59</v>
       </c>
       <c r="R24" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="S24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="T24" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="U24" t="s">
+        <v>59</v>
+      </c>
+      <c r="V24" t="s">
+        <v>59</v>
+      </c>
+      <c r="W24" t="s">
+        <v>59</v>
+      </c>
+      <c r="X24" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>59</v>
       </c>
       <c r="AB24" t="s">
         <v>59</v>
@@ -3044,38 +3488,83 @@
       <c r="A25" t="s">
         <v>49</v>
       </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="E25" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="F25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" t="s">
+        <v>59</v>
       </c>
       <c r="H25" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+      <c r="I25" t="s">
+        <v>59</v>
+      </c>
+      <c r="J25" t="s">
+        <v>59</v>
       </c>
       <c r="K25" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="L25" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="M25" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="N25" t="s">
+        <v>59</v>
       </c>
       <c r="O25" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="P25" t="s">
+        <v>59</v>
       </c>
       <c r="Q25" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="R25" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="S25" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="T25" t="s">
+        <v>59</v>
       </c>
       <c r="U25" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="V25" t="s">
+        <v>59</v>
+      </c>
+      <c r="W25" t="s">
+        <v>59</v>
+      </c>
+      <c r="X25" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>59</v>
       </c>
       <c r="AB25" t="s">
         <v>59</v>
@@ -3097,38 +3586,83 @@
       <c r="A26" t="s">
         <v>40</v>
       </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="E26" t="s">
+        <v>59</v>
       </c>
       <c r="F26" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="G26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H26" t="s">
+        <v>59</v>
       </c>
       <c r="I26" t="s">
-        <v>32</v>
+        <v>59</v>
+      </c>
+      <c r="J26" t="s">
+        <v>59</v>
+      </c>
+      <c r="K26" t="s">
+        <v>59</v>
       </c>
       <c r="L26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N26" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+      <c r="O26" t="s">
+        <v>59</v>
+      </c>
+      <c r="P26" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>59</v>
+      </c>
+      <c r="R26" t="s">
+        <v>59</v>
+      </c>
+      <c r="S26" t="s">
+        <v>59</v>
+      </c>
+      <c r="T26" t="s">
+        <v>59</v>
       </c>
       <c r="U26" t="s">
-        <v>49</v>
+        <v>59</v>
+      </c>
+      <c r="V26" t="s">
+        <v>59</v>
+      </c>
+      <c r="W26" t="s">
+        <v>59</v>
       </c>
       <c r="X26" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="Y26" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="Z26" t="s">
-        <v>50</v>
+        <v>59</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>59</v>
       </c>
       <c r="AB26" t="s">
         <v>59</v>
@@ -3150,44 +3684,83 @@
       <c r="A27" t="s">
         <v>54</v>
       </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="F27" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" t="s">
+        <v>59</v>
+      </c>
+      <c r="H27" t="s">
+        <v>59</v>
       </c>
       <c r="I27" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="J27" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="K27" t="s">
+        <v>59</v>
+      </c>
+      <c r="L27" t="s">
+        <v>59</v>
       </c>
       <c r="M27" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+      <c r="N27" t="s">
+        <v>59</v>
+      </c>
+      <c r="O27" t="s">
+        <v>59</v>
+      </c>
+      <c r="P27" t="s">
+        <v>59</v>
       </c>
       <c r="Q27" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="R27" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="S27" t="s">
+        <v>59</v>
       </c>
       <c r="T27" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="U27" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="V27" t="s">
+        <v>59</v>
       </c>
       <c r="W27" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="X27" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="Y27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z27" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>59</v>
       </c>
       <c r="AB27" t="s">
         <v>59</v>
@@ -3210,34 +3783,82 @@
         <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="E28" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" t="s">
+        <v>59</v>
+      </c>
+      <c r="H28" t="s">
+        <v>59</v>
+      </c>
+      <c r="I28" t="s">
+        <v>59</v>
+      </c>
+      <c r="J28" t="s">
+        <v>59</v>
       </c>
       <c r="K28" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="L28" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="M28" t="s">
+        <v>59</v>
+      </c>
+      <c r="N28" t="s">
+        <v>59</v>
+      </c>
+      <c r="O28" t="s">
+        <v>59</v>
       </c>
       <c r="P28" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="Q28" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="R28" t="s">
+        <v>59</v>
+      </c>
+      <c r="S28" t="s">
+        <v>59</v>
       </c>
       <c r="T28" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+      <c r="U28" t="s">
+        <v>59</v>
+      </c>
+      <c r="V28" t="s">
+        <v>59</v>
+      </c>
+      <c r="W28" t="s">
+        <v>59</v>
       </c>
       <c r="X28" t="s">
-        <v>50</v>
+        <v>59</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>59</v>
       </c>
       <c r="Z28" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>59</v>
       </c>
       <c r="AB28" t="s">
         <v>59</v>
@@ -3260,37 +3881,82 @@
         <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E29" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="F29" t="s">
+        <v>59</v>
+      </c>
+      <c r="G29" t="s">
+        <v>59</v>
       </c>
       <c r="H29" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="I29" t="s">
+        <v>59</v>
+      </c>
+      <c r="J29" t="s">
+        <v>59</v>
+      </c>
+      <c r="K29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L29" t="s">
+        <v>59</v>
       </c>
       <c r="M29" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="N29" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="O29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>59</v>
       </c>
       <c r="R29" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="S29" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="T29" t="s">
+        <v>59</v>
+      </c>
+      <c r="U29" t="s">
+        <v>59</v>
       </c>
       <c r="V29" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+      <c r="W29" t="s">
+        <v>59</v>
+      </c>
+      <c r="X29" t="s">
+        <v>59</v>
       </c>
       <c r="Y29" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="Z29" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>59</v>
       </c>
       <c r="AB29" t="s">
         <v>59</v>
@@ -3312,35 +3978,83 @@
       <c r="A30" t="s">
         <v>45</v>
       </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="D30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" t="s">
+        <v>59</v>
       </c>
       <c r="H30" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="I30" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="J30" t="s">
+        <v>59</v>
       </c>
       <c r="K30" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="L30" t="s">
+        <v>59</v>
+      </c>
+      <c r="M30" t="s">
+        <v>59</v>
       </c>
       <c r="N30" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="O30" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="P30" t="s">
+        <v>59</v>
       </c>
       <c r="Q30" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="R30" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="S30" t="s">
+        <v>59</v>
+      </c>
+      <c r="T30" t="s">
+        <v>59</v>
+      </c>
+      <c r="U30" t="s">
+        <v>59</v>
+      </c>
+      <c r="V30" t="s">
+        <v>59</v>
+      </c>
+      <c r="W30" t="s">
+        <v>59</v>
+      </c>
+      <c r="X30" t="s">
+        <v>59</v>
       </c>
       <c r="Y30" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="Z30" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>59</v>
       </c>
       <c r="AB30" t="s">
         <v>59</v>
@@ -3362,35 +4076,83 @@
       <c r="A31" t="s">
         <v>57</v>
       </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" t="s">
+        <v>59</v>
+      </c>
       <c r="H31" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="I31" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="J31" t="s">
+        <v>59</v>
+      </c>
+      <c r="K31" t="s">
+        <v>59</v>
+      </c>
+      <c r="L31" t="s">
+        <v>59</v>
       </c>
       <c r="M31" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="N31" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="O31" t="s">
+        <v>59</v>
+      </c>
+      <c r="P31" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>59</v>
       </c>
       <c r="R31" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="S31" t="s">
+        <v>59</v>
+      </c>
+      <c r="T31" t="s">
+        <v>59</v>
       </c>
       <c r="U31" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="V31" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="W31" t="s">
+        <v>59</v>
       </c>
       <c r="X31" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="Y31" t="s">
-        <v>32</v>
+        <v>59</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>59</v>
       </c>
       <c r="AA31" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AB31" t="s">
         <v>59</v>
@@ -3412,32 +4174,83 @@
       <c r="A32" t="s">
         <v>44</v>
       </c>
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
       <c r="C32" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" t="s">
+        <v>59</v>
+      </c>
+      <c r="F32" t="s">
+        <v>59</v>
       </c>
       <c r="G32" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="H32" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="I32" t="s">
+        <v>59</v>
+      </c>
+      <c r="J32" t="s">
+        <v>59</v>
+      </c>
+      <c r="K32" t="s">
+        <v>59</v>
+      </c>
+      <c r="L32" t="s">
+        <v>59</v>
       </c>
       <c r="M32" t="s">
-        <v>32</v>
+        <v>59</v>
+      </c>
+      <c r="N32" t="s">
+        <v>59</v>
+      </c>
+      <c r="O32" t="s">
+        <v>59</v>
       </c>
       <c r="P32" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q32" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="R32" t="s">
+        <v>59</v>
+      </c>
+      <c r="S32" t="s">
+        <v>59</v>
+      </c>
+      <c r="T32" t="s">
+        <v>59</v>
+      </c>
+      <c r="U32" t="s">
+        <v>59</v>
       </c>
       <c r="V32" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="W32" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="X32" t="s">
+        <v>59</v>
       </c>
       <c r="Y32" t="s">
-        <v>42</v>
+        <v>59</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>59</v>
       </c>
       <c r="AB32" t="s">
         <v>59</v>
@@ -3459,32 +4272,83 @@
       <c r="A33" t="s">
         <v>35</v>
       </c>
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" t="s">
+        <v>59</v>
+      </c>
       <c r="D33" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="E33" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="F33" t="s">
+        <v>59</v>
       </c>
       <c r="G33" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H33" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="I33" t="s">
+        <v>59</v>
+      </c>
+      <c r="J33" t="s">
+        <v>59</v>
+      </c>
+      <c r="K33" t="s">
+        <v>59</v>
+      </c>
+      <c r="L33" t="s">
+        <v>59</v>
+      </c>
+      <c r="M33" t="s">
+        <v>59</v>
       </c>
       <c r="N33" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="O33" t="s">
+        <v>59</v>
+      </c>
+      <c r="P33" t="s">
+        <v>59</v>
       </c>
       <c r="Q33" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="R33" t="s">
+        <v>59</v>
+      </c>
+      <c r="S33" t="s">
+        <v>59</v>
+      </c>
+      <c r="T33" t="s">
+        <v>59</v>
       </c>
       <c r="U33" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="V33" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="W33" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="X33" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>59</v>
       </c>
       <c r="AB33" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
randomize order and opponents
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\schedule_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35792C39-C97B-403E-90D0-24E8F15CA6EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3906345A-C31D-44C6-B62D-A0498CC6B767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,9 +127,6 @@
     <t>OAK</t>
   </si>
   <si>
-    <t>VAN</t>
-  </si>
-  <si>
     <t>NJ</t>
   </si>
   <si>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>DET</t>
+  </si>
+  <si>
+    <t>BAL</t>
   </si>
 </sst>
 </file>
@@ -1125,9 +1125,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H18" sqref="H18"/>
+      <selection pane="topRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1235,1567 +1235,1567 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
         <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
         <v>64</v>
       </c>
-      <c r="B12" t="s">
-        <v>59</v>
-      </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.3">
@@ -2803,391 +2803,391 @@
         <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.3">
@@ -3195,1175 +3195,1175 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>